<commit_message>
Updated JPN model - 2025-08-07 15:43
</commit_message>
<xml_diff>
--- a/VerveStacks_JPN/SuppXLS/Scen_Par-NGFS.xlsx
+++ b/VerveStacks_JPN/SuppXLS/Scen_Par-NGFS.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Veda\Veda\Veda_models\vervestacks_models\VerveStacks_JPN\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F40B606C-7ECB-40CC-939D-41E410045860}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{5A8F7EFA-D5B9-4BB7-8B8E-A52B8096BD8C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="17475" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2783,7 +2783,7 @@
   <dimension ref="B2:AA34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="Q10" sqref="Q10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -2852,7 +2852,7 @@
         <v>3</v>
       </c>
       <c r="Q10" s="3">
-        <f>SUMIFS(historical_data_long!$D$3:$D$9999,historical_data_long!$B$3:$B$9999,Veda!Q9,historical_data_long!$C$3:$C$9999,"TWh")</f>
+        <f>SUMIFS(historical_data_long!$D$3:$D$9999,historical_data_long!$B$3:$B$9999,Veda!Q9,historical_data_long!$C$3:$C$9999,"TWh")-R25+R26</f>
         <v>1040.57</v>
       </c>
       <c r="R10" s="2" t="s">

</xml_diff>